<commit_message>
two more test scripts for mixed membership functions for FIS rel, updated rule base of rel
</commit_message>
<xml_diff>
--- a/FIS/rel/rel_tests/rel_gauss/rel_gaussmf_output.xlsx
+++ b/FIS/rel/rel_tests/rel_gauss/rel_gaussmf_output.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Desktop\Final Year\Fuzzy_logic\cw\rel_tests\rel_gauss\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Desktop\fuzzy_cw\rel_tests\rel_gauss\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E97D08B6-6D9C-4918-9723-125BBC3189FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D21C9F34-9588-40EE-8DF8-15E7B9C71304}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="9765" xr2:uid="{DBAF3CF5-2B12-4B32-92E1-38786DB43149}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="12150" windowHeight="19215" xr2:uid="{DBAF3CF5-2B12-4B32-92E1-38786DB43149}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -436,7 +436,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F47A6EED-6893-42AF-8732-525F9B88C4C7}">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
@@ -464,7 +464,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>6.3104613751043992</v>
+        <v>6.2920276419332239</v>
       </c>
       <c r="B2">
         <v>6.3</v>
@@ -484,7 +484,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>6.211621830408447</v>
+        <v>6.0490642775245593</v>
       </c>
       <c r="B3">
         <v>6.23</v>
@@ -504,16 +504,16 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>5.6489976414534233</v>
+        <v>4.7342902645750051</v>
       </c>
       <c r="B4">
-        <v>5.67</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="C4">
-        <v>5.7049999999999992</v>
+        <v>4.871999999999999</v>
       </c>
       <c r="D4">
-        <v>4.41</v>
+        <v>2.4500000000000002</v>
       </c>
       <c r="E4">
         <v>7</v>
@@ -524,16 +524,16 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>5.0280139740362442</v>
+        <v>4.0146724957974183</v>
       </c>
       <c r="B5">
-        <v>5.04</v>
+        <v>4.2</v>
       </c>
       <c r="C5">
-        <v>5.004999999999999</v>
+        <v>4.0508695652173898</v>
       </c>
       <c r="D5">
-        <v>4.62</v>
+        <v>2.66</v>
       </c>
       <c r="E5">
         <v>5.39</v>
@@ -544,16 +544,16 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>4.9739753719962838</v>
+        <v>3.9453446815050182</v>
       </c>
       <c r="B6">
-        <v>4.97</v>
+        <v>3.64</v>
       </c>
       <c r="C6">
-        <v>5.004999999999999</v>
+        <v>4.0981818181818177</v>
       </c>
       <c r="D6">
-        <v>4.83</v>
+        <v>2.87</v>
       </c>
       <c r="E6">
         <v>5.18</v>
@@ -564,19 +564,19 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>4.9169085547969384</v>
+        <v>3.8198181722706677</v>
       </c>
       <c r="B7">
-        <v>4.97</v>
+        <v>3.43</v>
       </c>
       <c r="C7">
-        <v>4.97</v>
+        <v>3.01</v>
       </c>
       <c r="D7">
-        <v>4.97</v>
+        <v>3.01</v>
       </c>
       <c r="E7">
-        <v>4.97</v>
+        <v>3.01</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>9</v>
@@ -584,16 +584,16 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>4.7865346320171502</v>
+        <v>3.5034182301568149</v>
       </c>
       <c r="B8">
-        <v>4.9000000000000004</v>
+        <v>3.29</v>
       </c>
       <c r="C8">
-        <v>5.004999999999999</v>
+        <v>4.0981818181818177</v>
       </c>
       <c r="D8">
-        <v>4.83</v>
+        <v>2.87</v>
       </c>
       <c r="E8">
         <v>5.18</v>
@@ -604,16 +604,16 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>4.5315243808636474</v>
+        <v>2.7812219848714714</v>
       </c>
       <c r="B9">
-        <v>4.55</v>
+        <v>2.87</v>
       </c>
       <c r="C9">
-        <v>5.004999999999999</v>
+        <v>4.0508695652173898</v>
       </c>
       <c r="D9">
-        <v>4.62</v>
+        <v>2.66</v>
       </c>
       <c r="E9">
         <v>5.39</v>
@@ -624,19 +624,19 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>4.2200207510404768</v>
+        <v>1.9911650048790033</v>
       </c>
       <c r="B10">
-        <v>4.13</v>
+        <v>1.4</v>
       </c>
       <c r="C10">
-        <v>4.0250000000000004</v>
+        <v>1.3248148148148147</v>
       </c>
       <c r="D10">
-        <v>3.78</v>
+        <v>0</v>
       </c>
       <c r="E10">
-        <v>4.2699999999999996</v>
+        <v>3.22</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>11</v>
@@ -644,19 +644,19 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>4.0525338485577267</v>
+        <v>1.6128359075221363</v>
       </c>
       <c r="B11">
-        <v>3.99</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="C11">
-        <v>4.0249999999999995</v>
+        <v>1.02</v>
       </c>
       <c r="D11">
-        <v>3.92</v>
+        <v>0</v>
       </c>
       <c r="E11">
-        <v>4.13</v>
+        <v>3.08</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>11</v>
@@ -664,19 +664,19 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>4.0080972860772821</v>
+        <v>1.5026277781444826</v>
       </c>
       <c r="B12">
-        <v>3.99</v>
+        <v>1.05</v>
       </c>
       <c r="C12">
-        <v>3.99</v>
+        <v>0.64749999999999996</v>
       </c>
       <c r="D12">
-        <v>3.99</v>
+        <v>0</v>
       </c>
       <c r="E12">
-        <v>3.99</v>
+        <v>3.01</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>11</v>
@@ -684,19 +684,19 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>2.9918953272296394</v>
+        <v>3.9918979353713615</v>
       </c>
       <c r="B13">
-        <v>3.01</v>
+        <v>3.99</v>
       </c>
       <c r="C13">
-        <v>3.01</v>
+        <v>3.99</v>
       </c>
       <c r="D13">
-        <v>3.01</v>
+        <v>3.99</v>
       </c>
       <c r="E13">
-        <v>3.01</v>
+        <v>3.99</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>9</v>
@@ -704,19 +704,19 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>2.9911751381483191</v>
+        <v>3.9915858906130106</v>
       </c>
       <c r="B14">
-        <v>3.01</v>
+        <v>3.99</v>
       </c>
       <c r="C14">
-        <v>3.0100000000000002</v>
+        <v>3.99</v>
       </c>
       <c r="D14">
-        <v>2.87</v>
+        <v>3.85</v>
       </c>
       <c r="E14">
-        <v>3.15</v>
+        <v>4.13</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>9</v>
@@ -724,19 +724,19 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>3.004181146571693</v>
+        <v>3.9942603905120166</v>
       </c>
       <c r="B15">
-        <v>3.01</v>
+        <v>3.99</v>
       </c>
       <c r="C15">
-        <v>3.0100000000000002</v>
+        <v>3.99</v>
       </c>
       <c r="D15">
-        <v>2.66</v>
+        <v>3.64</v>
       </c>
       <c r="E15">
-        <v>3.36</v>
+        <v>4.34</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>8</v>
@@ -744,19 +744,19 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>3.6540879800725428</v>
+        <v>4.2899705318464783</v>
       </c>
       <c r="B16">
-        <v>3.36</v>
+        <v>4.2</v>
       </c>
       <c r="C16">
-        <v>3.01</v>
+        <v>3.9900000000000007</v>
       </c>
       <c r="D16">
-        <v>2.4500000000000002</v>
+        <v>3.43</v>
       </c>
       <c r="E16">
-        <v>3.57</v>
+        <v>4.55</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>8</v>
@@ -764,7 +764,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>4.8031182326189974</v>
+        <v>4.9123790596025163</v>
       </c>
       <c r="B17">
         <v>4.97</v>
@@ -784,7 +784,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>4.9684303286215146</v>
+        <v>4.9863967766256838</v>
       </c>
       <c r="B18">
         <v>4.97</v>
@@ -804,7 +804,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>5.0686218254843807</v>
+        <v>5.0546361570371774</v>
       </c>
       <c r="B19">
         <v>5.04</v>
@@ -824,7 +824,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>5.8143285317779876</v>
+        <v>5.7723631572360761</v>
       </c>
       <c r="B20">
         <v>5.88</v>
@@ -844,7 +844,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>6.208345972742543</v>
+        <v>6.1787883259107117</v>
       </c>
       <c r="B21">
         <v>6.23</v>
@@ -864,7 +864,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>6.2827136086732063</v>
+        <v>6.2609135440857155</v>
       </c>
       <c r="B22">
         <v>6.3</v>
@@ -884,16 +884,16 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>3.8971030497223818</v>
+        <v>3.3331391742079211</v>
       </c>
       <c r="B23">
-        <v>3.99</v>
+        <v>3.36</v>
       </c>
       <c r="C23">
-        <v>3.99</v>
+        <v>3.5</v>
       </c>
       <c r="D23">
-        <v>3.99</v>
+        <v>3.01</v>
       </c>
       <c r="E23">
         <v>3.99</v>
@@ -904,19 +904,19 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>2.5267567596665828</v>
+        <v>3.5067150619471064</v>
       </c>
       <c r="B24">
-        <v>2.52</v>
+        <v>3.5</v>
       </c>
       <c r="C24">
-        <v>2.5199999999999996</v>
+        <v>3.4999999999999996</v>
       </c>
       <c r="D24">
-        <v>1.47</v>
+        <v>2.4500000000000002</v>
       </c>
       <c r="E24">
-        <v>3.57</v>
+        <v>4.55</v>
       </c>
       <c r="G24" s="2" t="s">
         <v>9</v>
@@ -924,19 +924,19 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>3.7495556464509296</v>
+        <v>3.374803063316977</v>
       </c>
       <c r="B25">
-        <v>3.92</v>
+        <v>3.29</v>
       </c>
       <c r="C25">
-        <v>4.0250000000000004</v>
+        <v>3.0100000000000002</v>
       </c>
       <c r="D25">
-        <v>3.71</v>
+        <v>2.87</v>
       </c>
       <c r="E25">
-        <v>4.34</v>
+        <v>3.15</v>
       </c>
       <c r="G25" s="2" t="s">
         <v>9</v>
@@ -944,19 +944,19 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>3.7992412290106898</v>
+        <v>2.9455104173790643</v>
       </c>
       <c r="B26">
-        <v>3.85</v>
+        <v>3.08</v>
       </c>
       <c r="C26">
-        <v>4.0250000000000004</v>
+        <v>3.0100000000000002</v>
       </c>
       <c r="D26">
-        <v>3.71</v>
+        <v>2.87</v>
       </c>
       <c r="E26">
-        <v>4.34</v>
+        <v>3.15</v>
       </c>
       <c r="G26" s="2" t="s">
         <v>9</v>
@@ -964,19 +964,19 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>4.2711045210483158</v>
+        <v>1.8951320462239079</v>
       </c>
       <c r="B27">
-        <v>4.13</v>
+        <v>1.26</v>
       </c>
       <c r="C27">
-        <v>3.99</v>
+        <v>0.62999999999999989</v>
       </c>
       <c r="D27">
-        <v>3.64</v>
+        <v>0</v>
       </c>
       <c r="E27">
-        <v>4.34</v>
+        <v>1.26</v>
       </c>
       <c r="G27" s="2" t="s">
         <v>10</v>

</xml_diff>